<commit_message>
support formulas with 1 value ranges
</commit_message>
<xml_diff>
--- a/core/modules/core/test/smoketest/test1.xlsx
+++ b/core/modules/core/test/smoketest/test1.xlsx
@@ -193,7 +193,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -203,6 +202,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -505,42 +505,45 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13">
-        <f>SUM(A1:C1)</f>
-        <v>0</v>
+      <c r="D1" s="12" t="e">
+        <f>A1*C1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="14">
-        <f>SUM(A2:C2)</f>
-        <v>0</v>
+      <c r="D2" s="13" t="e">
+        <f>SUM(A2:C2)/A2</f>
+        <v>#VALUE!</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>1</v>
@@ -551,7 +554,7 @@
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="4">
@@ -563,16 +566,16 @@
     <row r="4" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1"/>

</xml_diff>